<commit_message>
poprawki na wysylanie do exela
</commit_message>
<xml_diff>
--- a/nowy_projekt/raport.xlsx
+++ b/nowy_projekt/raport.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,123 +468,139 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Soccer, Myanmar - National League</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sagaing United - Shan United FC</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 2.0</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1,83 → 1,46 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>2,16 → 1,89 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>↓↓↓ (over)</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Soccer, Myanmar - National League</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sagaing United - Shan United FC</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 2.0</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1,83 → 1,46 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>2,16 → 1,89 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>↓↓↓ (over)</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ballarat Rush - Ringwood Hawks</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 15.5</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2,27 → 1,60 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>2,16 → 1,89 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>↓↓↓ (over)</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ballarat Rush - Ringwood Hawks</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 15.5</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2,27 → 1,60 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>2,16 → 1,89 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>↓↓↓ (over)</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sandringham Sabres - Nunawading Spectres</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1st Half, 2-way</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3,78 → 2,84 ↓↓↓</t>
+          <t>2,16 → 1,89 ↓↓↓</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>↓↓↓ (away)</t>
+          <t>↓↓↓ (over)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>
@@ -592,50 +608,46 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sandringham Sabres - Nunawading Spectres</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1st Half, 2-way</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3,78 → 2,84 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>↓↓↓ (away)</t>
-        </is>
-      </c>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Basketball, Philippines - PBA on Tour</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Converge Fiberxers - Rain or Shine Elasto Painters</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 5.5</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1,91 → 1,69 ↓↓↓</t>
+          <t>2,29 → 1,76 ↓↓↓</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -644,22 +656,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Basketball, Philippines - PBA on Tour</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Converge Fiberxers - Rain or Shine Elasto Painters</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 5.5</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1,91 → 1,69 ↓↓↓</t>
+          <t>2,29 → 1,76 ↓↓↓</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -668,22 +680,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Soccer, Australia - NPL New South Wales</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Wollongong Wolves FC - St George City FA</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 0.5</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2,30 → 1,91 ↓↓↓</t>
+          <t>2,29 → 1,76 ↓↓↓</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -692,22 +704,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Soccer, Australia - NPL New South Wales</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wollongong Wolves FC - St George City FA</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap 0.5</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2,30 → 1,91 ↓↓↓</t>
+          <t>1,63 → 1,90</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -716,22 +728,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sandringham Sabres - Nunawading Spectres</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap -10.0</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2,40 → 1,60 ↓↓↓</t>
+          <t>1,63 → 1,90</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -740,22 +752,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Club Friendlies</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sandringham Sabres - Nunawading Spectres</t>
+          <t>Sparta Prague - FC Vysocina Jihlava</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap -10.0</t>
+          <t>Full time, (total) Under 4.0 / Over 4.0</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2,40 → 1,60 ↓↓↓</t>
+          <t>1,63 → 1,90</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -764,202 +776,582 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Soccer, Australia - NPL New South Wales</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sydney FC - Sydney United 58</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Full time, 3-way</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3,43 → 2,73 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>↓↓↓ (away)</t>
-        </is>
-      </c>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Soccer, Australia - NPL New South Wales</t>
+          <t>Basketball, Australia - NBL1 Women</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sydney FC - Sydney United 58</t>
+          <t>Perth Redbacks - Warwick Senators</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Full time, 3-way</t>
+          <t>Full time, Asian Handicap 34.5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3,43 → 2,73 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>↓↓↓ (away)</t>
-        </is>
-      </c>
+          <t>2,06 → 1,67 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Geelong Supercats - Melbourne Tigers</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap -23.0</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2,33 → 1,95 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1 Women</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Geelong Supercats - Melbourne Tigers</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Full time, Asian Handicap -23.0</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2,33 → 1,95 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Ballarat Miners - Ringwood Hawks</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Full time, (total) Under 190.5 / Over 190.5</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2,14 → 1,92 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ballarat Miners - Ringwood Hawks</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Full time, (total) Under 190.5 / Over 190.5</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2,14 → 1,92 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1</t>
+          <t>Soccer, Australia - NPL South Australia Women</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Townsville Heat - Rockhampton Rockets</t>
+          <t>Adelaide City - Fulham United</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Full time, (total) Under 187.0 / Over 187.0</t>
+          <t>Full time, Asian Handicap -2.5</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1,94 → 1,73 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Basketball, Australia - NBL1</t>
+          <t>Basketball, Australia - NBL1 Women</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Townsville Heat - Rockhampton Rockets</t>
+          <t>Perth Redbacks - Warwick Senators</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Full time, (total) Under 187.0 / Over 187.0</t>
+          <t>Full time, Asian Handicap 34.5</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1,94 → 1,73 ↓↓↓</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
+          <t>2,06 → 1,67 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Basketball, Australia - NBL1 Women</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Perth Redbacks - Warwick Senators</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap 34.5</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2,06 → 1,67 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1,49 → 1,97</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL New South Wales</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sydney FC - Sydney United 58</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Full time, 3-way</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1,83 → 2,19</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL New South Wales</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Wollongong Wolves FC - St George City FA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap 0.5</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1,62 → 1,77</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL New South Wales</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Wollongong Wolves FC - St George City FA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap 0.5</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1,62 → 1,77</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL New South Wales</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Wollongong Wolves FC - St George City FA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap 0.5</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2,30 → 1,91 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>↓↓↓ (away)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>↓↓↓ (away)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Soccer, Australia - NPL South Australia Women</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Adelaide City - Fulham United</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Full time, Asian Handicap -2.5</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2,29 → 1,76 ↓↓↓</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>↓↓↓ (home)</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>